<commit_message>
working successfully on mastermodule
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testdata.xlsx
+++ b/src/test/resources/TestData/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FromMacAdvancedFramework\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PSMSonNewFrameworkWindows\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C747C0FF-BB6C-44B7-A70F-F1325713D37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6349D8C-2AB6-4A08-BCFA-835BE9746C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" activeTab="1" xr2:uid="{1653A0DB-C2E4-5F45-84C3-178702117217}"/>
+    <workbookView xWindow="4200" yWindow="1815" windowWidth="15300" windowHeight="7875" xr2:uid="{1653A0DB-C2E4-5F45-84C3-178702117217}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Yes</t>
   </si>
@@ -58,22 +58,13 @@
     <t>demoTest</t>
   </si>
   <si>
-    <t>loginTest</t>
-  </si>
-  <si>
-    <t>logoutTest</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>masterModuleTest</t>
   </si>
 </sst>
 </file>
@@ -426,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F37FFB-6350-9941-B84F-5466CB090748}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -456,44 +447,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -506,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8572C43-C665-1D44-BF38-529E73A74250}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -534,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>

</xml_diff>